<commit_message>
cerca anche nella posizione definizione
</commit_message>
<xml_diff>
--- a/static/saved_dataframes/missing_columns_glossary_file.xlsx
+++ b/static/saved_dataframes/missing_columns_glossary_file.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1287,168 +1287,6 @@
         </is>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" s="2" t="n">
-        <v>43878</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>glossario_prova_1_0051</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>show</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" s="2" t="n">
-        <v>43878</v>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>glossario_prova_1_0052</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>show</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="B54" s="2" t="n">
-        <v>43878</v>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>glossario_prova_1_0053</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>show</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>53</v>
-      </c>
-      <c r="B55" s="2" t="n">
-        <v>43878</v>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>glossario_prova_1_0054</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>show</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="B56" s="2" t="n">
-        <v>43878</v>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>glossario_prova_1_0055</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>show</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" s="2" t="n">
-        <v>43878</v>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>glossario_prova_1_0056</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>show</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" s="2" t="n">
-        <v>43878</v>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>glossario_prova_1_0057</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>show</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" s="2" t="n">
-        <v>43878</v>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>glossario_prova_1_0058</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>show</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" s="2" t="n">
-        <v>43878</v>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>glossario_prova_1_0059</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>show</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiunti algoritmi di riversamento cumulativi. fatta una prova per ottenere il nome di un glossario senza il percorso. tentativo fallito e forse residui nel modello. eliminata manualmente la migrazione in .py e .pyc
</commit_message>
<xml_diff>
--- a/static/saved_dataframes/missing_columns_glossary_file.xlsx
+++ b/static/saved_dataframes/missing_columns_glossary_file.xlsx
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD" numFmtId="165"/>
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -392,11 +392,11 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0001</t>
+          <t>ITCH15825573217259687</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -410,11 +410,11 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0002</t>
+          <t>ITCH15825573217259688</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -428,11 +428,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0003</t>
+          <t>ITCH15825573217259689</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -446,11 +446,11 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0004</t>
+          <t>ITCH15825573217259690</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -464,11 +464,11 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0005</t>
+          <t>ITCH15825573217259691</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -482,11 +482,11 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0006</t>
+          <t>ITCH15825573217259692</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -500,11 +500,11 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0007</t>
+          <t>ITCH15825573217259693</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -518,11 +518,11 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0008</t>
+          <t>ITCH15825573217259694</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -536,11 +536,11 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0009</t>
+          <t>ITCH15825573217259695</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -554,11 +554,11 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0010</t>
+          <t>ITCH15825573217259696</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -572,11 +572,11 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0011</t>
+          <t>ITCH15825573217259697</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -590,11 +590,11 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0012</t>
+          <t>ITCH15825573217259698</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -608,11 +608,11 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0013</t>
+          <t>ITCH15825573217259699</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -626,11 +626,11 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0014</t>
+          <t>ITCH15825573217259700</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -644,11 +644,11 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0015</t>
+          <t>ITCH15825573217259701</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -662,11 +662,11 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0016</t>
+          <t>ITCH15825573217259702</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -680,11 +680,11 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0017</t>
+          <t>ITCH15825573217259703</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -698,11 +698,11 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0018</t>
+          <t>ITCH15825573217259704</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -716,11 +716,11 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0019</t>
+          <t>ITCH15825573217259705</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -734,11 +734,11 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0020</t>
+          <t>ITCH15825573217259706</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -752,11 +752,11 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0021</t>
+          <t>ITCH15825573217259707</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -770,11 +770,11 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0022</t>
+          <t>ITCH15825573217259708</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -788,11 +788,11 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0023</t>
+          <t>ITCH15825573217259709</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -806,11 +806,11 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0024</t>
+          <t>ITCH15825573217259710</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -824,11 +824,11 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0025</t>
+          <t>ITCH15825573217259711</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -842,11 +842,11 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0026</t>
+          <t>ITCH15825573217259712</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -860,11 +860,11 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0027</t>
+          <t>ITCH15825573217259713</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -878,11 +878,11 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0028</t>
+          <t>ITCH15825573217259714</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -896,11 +896,11 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0029</t>
+          <t>ITCH15825573217259715</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -914,11 +914,11 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0030</t>
+          <t>ITCH15825573217259716</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -932,11 +932,11 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0031</t>
+          <t>ITCH15825573217259717</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -950,11 +950,11 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0032</t>
+          <t>ITCH15825573217259718</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -968,11 +968,11 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0033</t>
+          <t>ITCH15825573217259719</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -986,11 +986,11 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0034</t>
+          <t>ITCH15825573217259720</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1004,11 +1004,11 @@
         <v>34</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0035</t>
+          <t>ITCH15825573217259721</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1022,11 +1022,11 @@
         <v>35</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0036</t>
+          <t>ITCH15825573217259722</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1040,11 +1040,11 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0037</t>
+          <t>ITCH15825573217259723</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1058,11 +1058,11 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0038</t>
+          <t>ITCH15825573217259724</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1076,11 +1076,11 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0039</t>
+          <t>ITCH15825573217259725</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1094,11 +1094,11 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0040</t>
+          <t>ITCH15825573217259726</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1112,11 +1112,11 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0041</t>
+          <t>ITCH15825573217259727</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1130,11 +1130,11 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0042</t>
+          <t>ITCH15825573217259728</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1148,11 +1148,11 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0043</t>
+          <t>ITCH15825573217259729</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1166,11 +1166,11 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0044</t>
+          <t>ITCH15825573217259730</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1184,11 +1184,11 @@
         <v>44</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0045</t>
+          <t>ITCH15825573217259731</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1202,11 +1202,11 @@
         <v>45</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0046</t>
+          <t>ITCH15825573217259732</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1220,11 +1220,11 @@
         <v>46</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0047</t>
+          <t>ITCH15825573217259733</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1238,11 +1238,11 @@
         <v>47</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0048</t>
+          <t>ITCH15825573217259734</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1256,11 +1256,11 @@
         <v>48</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0049</t>
+          <t>ITCH15825573217259735</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1274,11 +1274,11 @@
         <v>49</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>43878</v>
+        <v>43538</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>glossario_prova_1_0050</t>
+          <t>ITCH15825573217259736</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">

</xml_diff>

<commit_message>
inverito ordine di foglio elettronico e pai in esporta terminologia
</commit_message>
<xml_diff>
--- a/static/saved_dataframes/missing_columns_glossary_file.xlsx
+++ b/static/saved_dataframes/missing_columns_glossary_file.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -59,12 +56,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -362,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -391,12 +387,14 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>43538</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2018-07-16</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ITCH15825573217259687</t>
+          <t>IDF1008618</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -409,12 +407,14 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>43538</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2018-07-16</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ITCH15825573217259688</t>
+          <t>IDF1008619</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -427,12 +427,14 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>43538</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2018-07-16</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ITCH15825573217259689</t>
+          <t>IDF1008620</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -445,12 +447,14 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>43538</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2018-07-16</t>
+        </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ITCH15825573217259690</t>
+          <t>IDF1008647</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -463,12 +467,14 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>43538</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2020-01-08</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ITCH15825573217259691</t>
+          <t>ITCH00041</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -481,12 +487,14 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="n">
-        <v>43538</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2020-01-08</t>
+        </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ITCH15825573217259692</t>
+          <t>IDF1006146</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -499,12 +507,14 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="n">
-        <v>43538</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2020-01-08</t>
+        </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ITCH15825573217259693</t>
+          <t>IDF1002712</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -517,12 +527,14 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="n">
-        <v>43538</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2020-01-08</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ITCH15825573217259694</t>
+          <t>IDF1003030</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -535,12 +547,14 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="n">
-        <v>43538</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2017-03-01</t>
+        </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ITCH15825573217259695</t>
+          <t>IDF1002766</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -553,12 +567,14 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="n">
-        <v>43538</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2020-01-08</t>
+        </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ITCH15825573217259696</t>
+          <t>IDF1002720</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -571,12 +587,14 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="n">
-        <v>43538</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2020-01-08</t>
+        </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ITCH15825573217259697</t>
+          <t>IDF1002236</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -589,12 +607,14 @@
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="n">
-        <v>43538</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2020-01-08</t>
+        </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ITCH15825573217259698</t>
+          <t>ITCH00039</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -607,12 +627,14 @@
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="n">
-        <v>43538</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2020-01-08</t>
+        </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ITCH15825573217259699</t>
+          <t>IDF1002238</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -625,12 +647,14 @@
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="n">
-        <v>43538</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2020-01-08</t>
+        </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ITCH15825573217259700</t>
+          <t>IDF1006757</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -643,12 +667,14 @@
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="n">
-        <v>43538</v>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2020-01-08</t>
+        </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ITCH15825573217259701</t>
+          <t>ITCH00043</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -661,12 +687,14 @@
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="2" t="n">
-        <v>43538</v>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2018-07-16</t>
+        </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ITCH15825573217259702</t>
+          <t>IDF1008621</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -679,12 +707,14 @@
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="n">
-        <v>43538</v>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2019-12-18</t>
+        </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ITCH15825573217259703</t>
+          <t>ITCH00026</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -697,12 +727,14 @@
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="n">
-        <v>43538</v>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2018-07-16</t>
+        </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ITCH15825573217259704</t>
+          <t>IDF1008622</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -715,12 +747,14 @@
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="n">
-        <v>43538</v>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2018-07-16</t>
+        </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ITCH15825573217259705</t>
+          <t>IDF1008623</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -733,12 +767,14 @@
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="n">
-        <v>43538</v>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2018-07-16</t>
+        </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ITCH15825573217259706</t>
+          <t>IDF1008624</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -751,12 +787,14 @@
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" s="2" t="n">
-        <v>43538</v>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2018-07-16</t>
+        </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ITCH15825573217259707</t>
+          <t>IDF1008625</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -769,12 +807,14 @@
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" s="2" t="n">
-        <v>43538</v>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2018-11-08</t>
+        </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ITCH15825573217259708</t>
+          <t>ITCH00012</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -787,12 +827,14 @@
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24" s="2" t="n">
-        <v>43538</v>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2019-11-05</t>
+        </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ITCH15825573217259709</t>
+          <t>ITCH00036</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -805,12 +847,14 @@
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="2" t="n">
-        <v>43538</v>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2017-02-27</t>
+        </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ITCH15825573217259710</t>
+          <t>IDF1002273</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -823,12 +867,14 @@
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26" s="2" t="n">
-        <v>43538</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2018-07-16</t>
+        </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ITCH15825573217259711</t>
+          <t>IDF1008627</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -841,12 +887,14 @@
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27" s="2" t="n">
-        <v>43538</v>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2018-07-16</t>
+        </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ITCH15825573217259712</t>
+          <t>IDF1008628</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -859,12 +907,14 @@
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B28" s="2" t="n">
-        <v>43538</v>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2018-07-16</t>
+        </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ITCH15825573217259713</t>
+          <t>IDF1008629</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -877,12 +927,14 @@
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B29" s="2" t="n">
-        <v>43538</v>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2019-07-10</t>
+        </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ITCH15825573217259714</t>
+          <t>ITCH00003</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -895,12 +947,14 @@
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B30" s="2" t="n">
-        <v>43538</v>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2019-12-16</t>
+        </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ITCH15825573217259715</t>
+          <t>ITCH00025</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -913,12 +967,14 @@
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31" s="2" t="n">
-        <v>43538</v>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2017-02-27</t>
+        </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ITCH15825573217259716</t>
+          <t>IDF1002283</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -931,12 +987,14 @@
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B32" s="2" t="n">
-        <v>43538</v>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2020-01-14</t>
+        </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ITCH15825573217259717</t>
+          <t>ITCH00033</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -949,12 +1007,14 @@
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33" s="2" t="n">
-        <v>43538</v>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2020-01-08</t>
+        </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ITCH15825573217259718</t>
+          <t>ITCH00037</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -967,12 +1027,14 @@
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34" s="2" t="n">
-        <v>43538</v>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2020-01-14</t>
+        </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>ITCH15825573217259719</t>
+          <t>ITCH00034</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -985,12 +1047,14 @@
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B35" s="2" t="n">
-        <v>43538</v>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2019-10-28</t>
+        </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ITCH15825573217259720</t>
+          <t>ITCH00010</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1003,12 +1067,14 @@
       <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B36" s="2" t="n">
-        <v>43538</v>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2019-09-23</t>
+        </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ITCH15825573217259721</t>
+          <t>ITCH00007</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1021,12 +1087,14 @@
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37" s="2" t="n">
-        <v>43538</v>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2018-01-19</t>
+        </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>ITCH15825573217259722</t>
+          <t>IDF1008675</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1039,12 +1107,14 @@
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38" s="2" t="n">
-        <v>43538</v>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2019-10-28</t>
+        </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>ITCH15825573217259723</t>
+          <t>ITCH00009</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1057,12 +1127,14 @@
       <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B39" s="2" t="n">
-        <v>43538</v>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2019-12-05</t>
+        </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ITCH15825573217259724</t>
+          <t>ITCH00035</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1075,12 +1147,14 @@
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B40" s="2" t="n">
-        <v>43538</v>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2019-10-29</t>
+        </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ITCH15825573217259725</t>
+          <t>ITCH00028</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1093,12 +1167,14 @@
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B41" s="2" t="n">
-        <v>43538</v>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2019-10-29</t>
+        </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ITCH15825573217259726</t>
+          <t>ITCH00016</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1111,12 +1187,14 @@
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B42" s="2" t="n">
-        <v>43538</v>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2019-10-29</t>
+        </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ITCH15825573217259727</t>
+          <t>ITCH00022</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1129,12 +1207,14 @@
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B43" s="2" t="n">
-        <v>43538</v>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2019-10-29</t>
+        </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ITCH15825573217259728</t>
+          <t>ITCH00017</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1147,12 +1227,14 @@
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B44" s="2" t="n">
-        <v>43538</v>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2019-07-10</t>
+        </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>ITCH15825573217259729</t>
+          <t>ITCH00001</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1165,12 +1247,14 @@
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B45" s="2" t="n">
-        <v>43538</v>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2019-07-10</t>
+        </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ITCH15825573217259730</t>
+          <t>ITCH00004</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1183,12 +1267,14 @@
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B46" s="2" t="n">
-        <v>43538</v>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2019-12-18</t>
+        </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>ITCH15825573217259731</t>
+          <t>ITCH00029</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1201,12 +1287,14 @@
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B47" s="2" t="n">
-        <v>43538</v>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2019-10-28</t>
+        </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ITCH15825573217259732</t>
+          <t>ITCH00014</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1219,12 +1307,14 @@
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B48" s="2" t="n">
-        <v>43538</v>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2019-07-11</t>
+        </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ITCH15825573217259733</t>
+          <t>ITCH00006</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1237,12 +1327,14 @@
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B49" s="2" t="n">
-        <v>43538</v>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2019-10-28</t>
+        </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ITCH15825573217259734</t>
+          <t>ITCH00013</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1255,12 +1347,14 @@
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B50" s="2" t="n">
-        <v>43538</v>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2019-07-11</t>
+        </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ITCH15825573217259735</t>
+          <t>ITCH00005</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1273,15 +1367,257 @@
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B51" s="2" t="n">
-        <v>43538</v>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2019-11-11</t>
+        </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>ITCH15825573217259736</t>
+          <t>ITCH00027</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2019-12-18</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>ITCH00031</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2019-10-28</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>ITCH00030</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2019-10-29</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>ITCH00018</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2019-10-28</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>ITCH00011</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>2019-10-29</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>ITCH00019</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2019-10-28</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>ITCH00015</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>2020-01-15</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>ITCH00032</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>2019-10-28</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>ITCH00021</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2019-10-29</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>ITCH00020</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>2019-10-29</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>ITCH00024</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>2019-07-10</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>ITCH00002</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>2019-10-29</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>ITCH00023</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
         <is>
           <t>show</t>
         </is>

</xml_diff>